<commit_message>
Pushing the latest changes
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/DataAnalytics.xlsx
+++ b/src/test/resources/TestData/DataAnalytics.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renita.lobo\DP-AIMM-QAAutomation\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DP-AIMM-QAAutomation\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD479529-40D3-4465-8238-5DA2698F0A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4740A8A2-5AF7-4D69-9170-D2800908A59D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A4CDE6D7-D9AB-4EF7-BE72-FD4E7A10679C}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Global" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DataAnalytics!$AZ$1:$AZ$193</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DataAnalytics!$BA$1:$BA$193</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>TC Name</t>
   </si>
@@ -96,9 +96,6 @@
     <t>productName2</t>
   </si>
   <si>
-    <t>Sauce Labs Bike Light</t>
-  </si>
-  <si>
     <t>firstName</t>
   </si>
   <si>
@@ -121,6 +118,15 @@
   </si>
   <si>
     <t>url</t>
+  </si>
+  <si>
+    <t>filterOption</t>
+  </si>
+  <si>
+    <t>Price (high to low)</t>
+  </si>
+  <si>
+    <t>Sauce Labs Fleece Jacket</t>
   </si>
 </sst>
 </file>
@@ -600,12 +606,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62FA245C-CBB2-414D-93CD-B52B807688EF}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:BB193"/>
+  <dimension ref="A1:BC193"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="R1" sqref="R1"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
@@ -614,70 +620,70 @@
     <col min="2" max="2" width="14.7265625" style="2" customWidth="1"/>
     <col min="3" max="3" width="26.36328125" style="2" customWidth="1"/>
     <col min="4" max="4" width="14.453125" style="2" customWidth="1"/>
-    <col min="5" max="6" width="14.1796875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="22.453125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="16" style="2" customWidth="1"/>
-    <col min="9" max="9" width="14.54296875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="20.453125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="16.6328125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="28.26953125" style="2" customWidth="1"/>
-    <col min="13" max="14" width="17.26953125" style="2" customWidth="1"/>
-    <col min="15" max="16" width="15.26953125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="23.453125" style="2" customWidth="1"/>
-    <col min="18" max="20" width="17.26953125" style="2" customWidth="1"/>
-    <col min="21" max="21" width="11.453125" style="2" customWidth="1"/>
-    <col min="22" max="22" width="9.7265625" style="2" customWidth="1"/>
-    <col min="23" max="23" width="8.1796875" style="2" customWidth="1"/>
-    <col min="24" max="25" width="7.26953125" style="2" customWidth="1"/>
-    <col min="26" max="26" width="9.1796875" style="2" customWidth="1"/>
-    <col min="27" max="27" width="10.81640625" style="2" customWidth="1"/>
-    <col min="28" max="28" width="17.26953125" style="2" customWidth="1"/>
-    <col min="29" max="29" width="22.453125" style="2" customWidth="1"/>
-    <col min="30" max="30" width="21.1796875" style="2" customWidth="1"/>
-    <col min="31" max="33" width="11.54296875" style="2" customWidth="1"/>
-    <col min="34" max="34" width="34.7265625" style="2" customWidth="1"/>
-    <col min="35" max="35" width="37.26953125" style="2" customWidth="1"/>
-    <col min="36" max="36" width="20.7265625" style="2" customWidth="1"/>
-    <col min="37" max="37" width="19.81640625" style="2" customWidth="1"/>
-    <col min="38" max="38" width="13.90625" style="2" customWidth="1"/>
-    <col min="39" max="39" width="13.7265625" style="2" customWidth="1"/>
-    <col min="40" max="40" width="13.36328125" style="2" customWidth="1"/>
-    <col min="41" max="41" width="16.1796875" style="2" customWidth="1"/>
-    <col min="42" max="42" width="16" style="2" customWidth="1"/>
-    <col min="43" max="43" width="16.1796875" style="2" customWidth="1"/>
-    <col min="44" max="44" width="30.54296875" style="2" customWidth="1"/>
-    <col min="45" max="45" width="13.90625" style="2" customWidth="1"/>
-    <col min="46" max="46" width="27.54296875" style="2" customWidth="1"/>
-    <col min="47" max="47" width="24.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="20" style="2" customWidth="1"/>
-    <col min="49" max="50" width="27" style="2" customWidth="1"/>
-    <col min="51" max="51" width="21.54296875" style="2" customWidth="1"/>
-    <col min="52" max="52" width="14.54296875" style="2" customWidth="1"/>
-    <col min="53" max="53" width="19.453125" style="2" customWidth="1"/>
-    <col min="54" max="54" width="24.54296875" style="2" customWidth="1"/>
-    <col min="55" max="55" width="27.1796875" style="2" customWidth="1"/>
-    <col min="56" max="56" width="22.7265625" style="2" customWidth="1"/>
-    <col min="57" max="57" width="20" style="2" customWidth="1"/>
-    <col min="58" max="58" width="15.1796875" style="2" customWidth="1"/>
-    <col min="59" max="59" width="21.1796875" style="2" customWidth="1"/>
-    <col min="60" max="60" width="12.26953125" style="2" customWidth="1"/>
-    <col min="61" max="61" width="12.81640625" style="2" customWidth="1"/>
-    <col min="62" max="62" width="18" style="2" customWidth="1"/>
-    <col min="63" max="63" width="25" style="2" customWidth="1"/>
-    <col min="64" max="64" width="18.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="15" style="2" customWidth="1"/>
-    <col min="66" max="66" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="29.54296875" style="2" customWidth="1"/>
-    <col min="68" max="68" width="26" style="2" customWidth="1"/>
-    <col min="69" max="69" width="20.81640625" style="2" customWidth="1"/>
-    <col min="70" max="70" width="17.26953125" style="2" customWidth="1"/>
-    <col min="71" max="71" width="25.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="19.1796875" style="2" customWidth="1"/>
-    <col min="73" max="73" width="21.1796875" style="2" customWidth="1"/>
-    <col min="74" max="16384" width="9.1796875" style="2"/>
+    <col min="5" max="7" width="14.1796875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="22.453125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="16" style="2" customWidth="1"/>
+    <col min="10" max="10" width="14.54296875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="20.453125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="16.6328125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="28.26953125" style="2" customWidth="1"/>
+    <col min="14" max="15" width="17.26953125" style="2" customWidth="1"/>
+    <col min="16" max="17" width="15.26953125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="23.453125" style="2" customWidth="1"/>
+    <col min="19" max="21" width="17.26953125" style="2" customWidth="1"/>
+    <col min="22" max="22" width="11.453125" style="2" customWidth="1"/>
+    <col min="23" max="23" width="9.7265625" style="2" customWidth="1"/>
+    <col min="24" max="24" width="8.1796875" style="2" customWidth="1"/>
+    <col min="25" max="26" width="7.26953125" style="2" customWidth="1"/>
+    <col min="27" max="27" width="9.1796875" style="2" customWidth="1"/>
+    <col min="28" max="28" width="10.81640625" style="2" customWidth="1"/>
+    <col min="29" max="29" width="17.26953125" style="2" customWidth="1"/>
+    <col min="30" max="30" width="22.453125" style="2" customWidth="1"/>
+    <col min="31" max="31" width="21.1796875" style="2" customWidth="1"/>
+    <col min="32" max="34" width="11.54296875" style="2" customWidth="1"/>
+    <col min="35" max="35" width="34.7265625" style="2" customWidth="1"/>
+    <col min="36" max="36" width="37.26953125" style="2" customWidth="1"/>
+    <col min="37" max="37" width="20.7265625" style="2" customWidth="1"/>
+    <col min="38" max="38" width="19.81640625" style="2" customWidth="1"/>
+    <col min="39" max="39" width="13.90625" style="2" customWidth="1"/>
+    <col min="40" max="40" width="13.7265625" style="2" customWidth="1"/>
+    <col min="41" max="41" width="13.36328125" style="2" customWidth="1"/>
+    <col min="42" max="42" width="16.1796875" style="2" customWidth="1"/>
+    <col min="43" max="43" width="16" style="2" customWidth="1"/>
+    <col min="44" max="44" width="16.1796875" style="2" customWidth="1"/>
+    <col min="45" max="45" width="30.54296875" style="2" customWidth="1"/>
+    <col min="46" max="46" width="13.90625" style="2" customWidth="1"/>
+    <col min="47" max="47" width="27.54296875" style="2" customWidth="1"/>
+    <col min="48" max="48" width="24.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="20" style="2" customWidth="1"/>
+    <col min="50" max="51" width="27" style="2" customWidth="1"/>
+    <col min="52" max="52" width="21.54296875" style="2" customWidth="1"/>
+    <col min="53" max="53" width="14.54296875" style="2" customWidth="1"/>
+    <col min="54" max="54" width="19.453125" style="2" customWidth="1"/>
+    <col min="55" max="55" width="24.54296875" style="2" customWidth="1"/>
+    <col min="56" max="56" width="27.1796875" style="2" customWidth="1"/>
+    <col min="57" max="57" width="22.7265625" style="2" customWidth="1"/>
+    <col min="58" max="58" width="20" style="2" customWidth="1"/>
+    <col min="59" max="59" width="15.1796875" style="2" customWidth="1"/>
+    <col min="60" max="60" width="21.1796875" style="2" customWidth="1"/>
+    <col min="61" max="61" width="12.26953125" style="2" customWidth="1"/>
+    <col min="62" max="62" width="12.81640625" style="2" customWidth="1"/>
+    <col min="63" max="63" width="18" style="2" customWidth="1"/>
+    <col min="64" max="64" width="25" style="2" customWidth="1"/>
+    <col min="65" max="65" width="18.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="15" style="2" customWidth="1"/>
+    <col min="67" max="67" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="29.54296875" style="2" customWidth="1"/>
+    <col min="69" max="69" width="26" style="2" customWidth="1"/>
+    <col min="70" max="70" width="20.81640625" style="2" customWidth="1"/>
+    <col min="71" max="71" width="17.26953125" style="2" customWidth="1"/>
+    <col min="72" max="72" width="25.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="19.1796875" style="2" customWidth="1"/>
+    <col min="74" max="74" width="21.1796875" style="2" customWidth="1"/>
+    <col min="75" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="1" customFormat="1" ht="34.5" customHeight="1">
+    <row r="1" spans="1:38" s="1" customFormat="1" ht="34.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -685,7 +691,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>9</v>
@@ -697,22 +703,25 @@
         <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:37" ht="35" customHeight="1">
+    </row>
+    <row r="2" spans="1:38" ht="35" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -720,7 +729,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>10</v>
@@ -732,21 +741,23 @@
         <v>15</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="5"/>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
@@ -755,20 +766,21 @@
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
-      <c r="U2" s="3"/>
+      <c r="U2" s="5"/>
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
-      <c r="X2" s="6"/>
+      <c r="X2" s="3"/>
       <c r="Y2" s="6"/>
       <c r="Z2" s="6"/>
-      <c r="AJ2" s="4"/>
+      <c r="AA2" s="6"/>
       <c r="AK2" s="4"/>
-    </row>
-    <row r="15" spans="1:37" ht="14.5">
-      <c r="G15" s="5"/>
+      <c r="AL2" s="4"/>
+    </row>
+    <row r="15" spans="1:38" ht="14.5">
       <c r="H15" s="5"/>
-    </row>
-    <row r="180" spans="5:54" ht="14.5">
+      <c r="I15" s="5"/>
+    </row>
+    <row r="180" spans="5:55" ht="14.5">
       <c r="E180" s="3"/>
       <c r="F180" s="3"/>
       <c r="G180" s="3"/>
@@ -794,7 +806,7 @@
       <c r="AA180" s="3"/>
       <c r="AB180" s="3"/>
       <c r="AC180" s="3"/>
-      <c r="AU180" s="4"/>
+      <c r="AD180" s="3"/>
       <c r="AV180" s="4"/>
       <c r="AW180" s="4"/>
       <c r="AX180" s="4"/>
@@ -802,8 +814,9 @@
       <c r="AZ180" s="4"/>
       <c r="BA180" s="4"/>
       <c r="BB180" s="4"/>
-    </row>
-    <row r="181" spans="5:54" ht="14.5">
+      <c r="BC180" s="4"/>
+    </row>
+    <row r="181" spans="5:55" ht="14.5">
       <c r="E181" s="3"/>
       <c r="F181" s="3"/>
       <c r="G181" s="3"/>
@@ -829,7 +842,7 @@
       <c r="AA181" s="3"/>
       <c r="AB181" s="3"/>
       <c r="AC181" s="3"/>
-      <c r="AU181" s="4"/>
+      <c r="AD181" s="3"/>
       <c r="AV181" s="4"/>
       <c r="AW181" s="4"/>
       <c r="AX181" s="4"/>
@@ -837,8 +850,9 @@
       <c r="AZ181" s="4"/>
       <c r="BA181" s="4"/>
       <c r="BB181" s="4"/>
-    </row>
-    <row r="182" spans="5:54" ht="14.5">
+      <c r="BC181" s="4"/>
+    </row>
+    <row r="182" spans="5:55" ht="14.5">
       <c r="E182" s="3"/>
       <c r="F182" s="3"/>
       <c r="G182" s="3"/>
@@ -864,7 +878,7 @@
       <c r="AA182" s="3"/>
       <c r="AB182" s="3"/>
       <c r="AC182" s="3"/>
-      <c r="AU182" s="4"/>
+      <c r="AD182" s="3"/>
       <c r="AV182" s="4"/>
       <c r="AW182" s="4"/>
       <c r="AX182" s="4"/>
@@ -872,8 +886,9 @@
       <c r="AZ182" s="4"/>
       <c r="BA182" s="4"/>
       <c r="BB182" s="4"/>
-    </row>
-    <row r="183" spans="5:54" ht="14.5">
+      <c r="BC182" s="4"/>
+    </row>
+    <row r="183" spans="5:55" ht="14.5">
       <c r="E183" s="3"/>
       <c r="F183" s="3"/>
       <c r="G183" s="3"/>
@@ -899,7 +914,7 @@
       <c r="AA183" s="3"/>
       <c r="AB183" s="3"/>
       <c r="AC183" s="3"/>
-      <c r="AU183" s="4"/>
+      <c r="AD183" s="3"/>
       <c r="AV183" s="4"/>
       <c r="AW183" s="4"/>
       <c r="AX183" s="4"/>
@@ -907,8 +922,9 @@
       <c r="AZ183" s="4"/>
       <c r="BA183" s="4"/>
       <c r="BB183" s="4"/>
-    </row>
-    <row r="184" spans="5:54" ht="14.5">
+      <c r="BC183" s="4"/>
+    </row>
+    <row r="184" spans="5:55" ht="14.5">
       <c r="E184" s="3"/>
       <c r="F184" s="3"/>
       <c r="G184" s="3"/>
@@ -934,7 +950,7 @@
       <c r="AA184" s="3"/>
       <c r="AB184" s="3"/>
       <c r="AC184" s="3"/>
-      <c r="AU184" s="4"/>
+      <c r="AD184" s="3"/>
       <c r="AV184" s="4"/>
       <c r="AW184" s="4"/>
       <c r="AX184" s="4"/>
@@ -942,8 +958,9 @@
       <c r="AZ184" s="4"/>
       <c r="BA184" s="4"/>
       <c r="BB184" s="4"/>
-    </row>
-    <row r="185" spans="5:54" ht="14.5">
+      <c r="BC184" s="4"/>
+    </row>
+    <row r="185" spans="5:55" ht="14.5">
       <c r="E185" s="3"/>
       <c r="F185" s="3"/>
       <c r="G185" s="3"/>
@@ -969,7 +986,7 @@
       <c r="AA185" s="3"/>
       <c r="AB185" s="3"/>
       <c r="AC185" s="3"/>
-      <c r="AU185" s="4"/>
+      <c r="AD185" s="3"/>
       <c r="AV185" s="4"/>
       <c r="AW185" s="4"/>
       <c r="AX185" s="4"/>
@@ -977,8 +994,9 @@
       <c r="AZ185" s="4"/>
       <c r="BA185" s="4"/>
       <c r="BB185" s="4"/>
-    </row>
-    <row r="186" spans="5:54" ht="14.5">
+      <c r="BC185" s="4"/>
+    </row>
+    <row r="186" spans="5:55" ht="14.5">
       <c r="E186" s="3"/>
       <c r="F186" s="3"/>
       <c r="G186" s="3"/>
@@ -1004,7 +1022,7 @@
       <c r="AA186" s="3"/>
       <c r="AB186" s="3"/>
       <c r="AC186" s="3"/>
-      <c r="AU186" s="4"/>
+      <c r="AD186" s="3"/>
       <c r="AV186" s="4"/>
       <c r="AW186" s="4"/>
       <c r="AX186" s="4"/>
@@ -1012,8 +1030,9 @@
       <c r="AZ186" s="4"/>
       <c r="BA186" s="4"/>
       <c r="BB186" s="4"/>
-    </row>
-    <row r="187" spans="5:54" ht="14.5">
+      <c r="BC186" s="4"/>
+    </row>
+    <row r="187" spans="5:55" ht="14.5">
       <c r="E187" s="3"/>
       <c r="F187" s="3"/>
       <c r="G187" s="3"/>
@@ -1039,7 +1058,7 @@
       <c r="AA187" s="3"/>
       <c r="AB187" s="3"/>
       <c r="AC187" s="3"/>
-      <c r="AU187" s="4"/>
+      <c r="AD187" s="3"/>
       <c r="AV187" s="4"/>
       <c r="AW187" s="4"/>
       <c r="AX187" s="4"/>
@@ -1047,8 +1066,9 @@
       <c r="AZ187" s="4"/>
       <c r="BA187" s="4"/>
       <c r="BB187" s="4"/>
-    </row>
-    <row r="188" spans="5:54" ht="14.5">
+      <c r="BC187" s="4"/>
+    </row>
+    <row r="188" spans="5:55" ht="14.5">
       <c r="E188" s="3"/>
       <c r="F188" s="3"/>
       <c r="G188" s="3"/>
@@ -1074,7 +1094,7 @@
       <c r="AA188" s="3"/>
       <c r="AB188" s="3"/>
       <c r="AC188" s="3"/>
-      <c r="AU188" s="4"/>
+      <c r="AD188" s="3"/>
       <c r="AV188" s="4"/>
       <c r="AW188" s="4"/>
       <c r="AX188" s="4"/>
@@ -1082,8 +1102,9 @@
       <c r="AZ188" s="4"/>
       <c r="BA188" s="4"/>
       <c r="BB188" s="4"/>
-    </row>
-    <row r="189" spans="5:54" ht="14.5">
+      <c r="BC188" s="4"/>
+    </row>
+    <row r="189" spans="5:55" ht="14.5">
       <c r="E189" s="3"/>
       <c r="F189" s="3"/>
       <c r="G189" s="3"/>
@@ -1109,7 +1130,7 @@
       <c r="AA189" s="3"/>
       <c r="AB189" s="3"/>
       <c r="AC189" s="3"/>
-      <c r="AU189" s="4"/>
+      <c r="AD189" s="3"/>
       <c r="AV189" s="4"/>
       <c r="AW189" s="4"/>
       <c r="AX189" s="4"/>
@@ -1117,8 +1138,9 @@
       <c r="AZ189" s="4"/>
       <c r="BA189" s="4"/>
       <c r="BB189" s="4"/>
-    </row>
-    <row r="190" spans="5:54" ht="14.5">
+      <c r="BC189" s="4"/>
+    </row>
+    <row r="190" spans="5:55" ht="14.5">
       <c r="E190" s="3"/>
       <c r="F190" s="3"/>
       <c r="G190" s="3"/>
@@ -1144,7 +1166,7 @@
       <c r="AA190" s="3"/>
       <c r="AB190" s="3"/>
       <c r="AC190" s="3"/>
-      <c r="AU190" s="4"/>
+      <c r="AD190" s="3"/>
       <c r="AV190" s="4"/>
       <c r="AW190" s="4"/>
       <c r="AX190" s="4"/>
@@ -1152,8 +1174,9 @@
       <c r="AZ190" s="4"/>
       <c r="BA190" s="4"/>
       <c r="BB190" s="4"/>
-    </row>
-    <row r="191" spans="5:54" ht="14.5">
+      <c r="BC190" s="4"/>
+    </row>
+    <row r="191" spans="5:55" ht="14.5">
       <c r="E191" s="3"/>
       <c r="F191" s="3"/>
       <c r="G191" s="3"/>
@@ -1179,7 +1202,7 @@
       <c r="AA191" s="3"/>
       <c r="AB191" s="3"/>
       <c r="AC191" s="3"/>
-      <c r="AU191" s="4"/>
+      <c r="AD191" s="3"/>
       <c r="AV191" s="4"/>
       <c r="AW191" s="4"/>
       <c r="AX191" s="4"/>
@@ -1187,8 +1210,9 @@
       <c r="AZ191" s="4"/>
       <c r="BA191" s="4"/>
       <c r="BB191" s="4"/>
-    </row>
-    <row r="192" spans="5:54" ht="14.5">
+      <c r="BC191" s="4"/>
+    </row>
+    <row r="192" spans="5:55" ht="14.5">
       <c r="E192" s="3"/>
       <c r="F192" s="3"/>
       <c r="G192" s="3"/>
@@ -1214,7 +1238,7 @@
       <c r="AA192" s="3"/>
       <c r="AB192" s="3"/>
       <c r="AC192" s="3"/>
-      <c r="AU192" s="4"/>
+      <c r="AD192" s="3"/>
       <c r="AV192" s="4"/>
       <c r="AW192" s="4"/>
       <c r="AX192" s="4"/>
@@ -1222,8 +1246,9 @@
       <c r="AZ192" s="4"/>
       <c r="BA192" s="4"/>
       <c r="BB192" s="4"/>
-    </row>
-    <row r="193" spans="5:54" ht="14.5">
+      <c r="BC192" s="4"/>
+    </row>
+    <row r="193" spans="5:55" ht="14.5">
       <c r="E193" s="3"/>
       <c r="F193" s="3"/>
       <c r="G193" s="3"/>
@@ -1249,7 +1274,7 @@
       <c r="AA193" s="3"/>
       <c r="AB193" s="3"/>
       <c r="AC193" s="3"/>
-      <c r="AU193" s="4"/>
+      <c r="AD193" s="3"/>
       <c r="AV193" s="4"/>
       <c r="AW193" s="4"/>
       <c r="AX193" s="4"/>
@@ -1257,6 +1282,7 @@
       <c r="AZ193" s="4"/>
       <c r="BA193" s="4"/>
       <c r="BB193" s="4"/>
+      <c r="BC193" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -1308,7 +1334,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -1325,7 +1351,7 @@
     </row>
     <row r="2" spans="1:5" s="4" customFormat="1" ht="27.5" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>2</v>

</xml_diff>